<commit_message>
funcionalidades 1 y 2 pasando test excel 3 metido
</commit_message>
<xml_diff>
--- a/GE3_TestCasesTemplate_v1.0.xlsx
+++ b/GE3_TestCasesTemplate_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Universidad\2\2oCuatrimestre\Desarrollo de Software\EjerciciosGuiados\EG3\G81.T17.EG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE643370-BA3D-4578-93B1-3F8EB424F48C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D6E76-DA20-4AB2-BDE4-4CB264A49175}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="19524" windowHeight="10308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>ID TEST</t>
   </si>
@@ -60,36 +60,15 @@
     <t>KEY</t>
   </si>
   <si>
-    <t>1_3_5_6_8_10</t>
-  </si>
-  <si>
     <t>12341321413241324132412341324132</t>
   </si>
   <si>
     <t>1_2_3_4_6_7</t>
   </si>
   <si>
-    <t>test_open_door_resident</t>
-  </si>
-  <si>
-    <t>test_open_door</t>
-  </si>
-  <si>
-    <t>1_2_3_4_6_8</t>
-  </si>
-  <si>
-    <t>test_open_door_bad</t>
-  </si>
-  <si>
-    <t>Camino considerando que encuentra la clave y residente (fecha 0)</t>
-  </si>
-  <si>
     <t>Camino considerando que encuentra la clave y no ha expirado</t>
   </si>
   <si>
-    <t>Camino considerando que encuentra la clave y no ha expirado (fecha menor fecha actual)</t>
-  </si>
-  <si>
     <t>Loop: 3_8</t>
   </si>
   <si>
@@ -99,12 +78,6 @@
     <t>Loop: 3_5_6_3_5_6</t>
   </si>
   <si>
-    <t>Loop: 3_5_6_(99)_8</t>
-  </si>
-  <si>
-    <t>Loop: 3_5_6_(100)_9</t>
-  </si>
-  <si>
     <t>loop_0_times</t>
   </si>
   <si>
@@ -114,15 +87,6 @@
     <t>loop_2_times</t>
   </si>
   <si>
-    <t>loop_99_times</t>
-  </si>
-  <si>
-    <t>loop_100_times</t>
-  </si>
-  <si>
-    <t>loop_101_times</t>
-  </si>
-  <si>
     <t>No entrar al loop</t>
   </si>
   <si>
@@ -132,13 +96,112 @@
     <t>Entrar 2 veces</t>
   </si>
   <si>
-    <t>Entrar 99 veces</t>
-  </si>
-  <si>
-    <t>Entrar 100 veces</t>
-  </si>
-  <si>
-    <t>Entrar 101 veces</t>
+    <t>1_2_3_8</t>
+  </si>
+  <si>
+    <t>1_2_3_4_5_7</t>
+  </si>
+  <si>
+    <t>1_2_3_4_5_8</t>
+  </si>
+  <si>
+    <t>1_2_3_4_8</t>
+  </si>
+  <si>
+    <t>1_2</t>
+  </si>
+  <si>
+    <t>1_3</t>
+  </si>
+  <si>
+    <t>1_2_5</t>
+  </si>
+  <si>
+    <t>1_4</t>
+  </si>
+  <si>
+    <t>Camino considerando que encuentra la clave y la fecha es 0</t>
+  </si>
+  <si>
+    <t>Camino considerando que encuentra la clave y ha expirado</t>
+  </si>
+  <si>
+    <t>Camino considerando que no encuentra la clave</t>
+  </si>
+  <si>
+    <t>Camino considerando que el fichero está vacío</t>
+  </si>
+  <si>
+    <t>test_open_door_no_clave</t>
+  </si>
+  <si>
+    <t>test_open_door_fichero_vacio</t>
+  </si>
+  <si>
+    <t>test_open_door_clave_no_exp</t>
+  </si>
+  <si>
+    <t>test_open_door_clave_fecha_0</t>
+  </si>
+  <si>
+    <t>test_open_door_clave_exp</t>
+  </si>
+  <si>
+    <t>Abrir fichero y leer datos</t>
+  </si>
+  <si>
+    <t>Fichero no encontrado</t>
+  </si>
+  <si>
+    <t>test_check_key_clave_valida</t>
+  </si>
+  <si>
+    <t>test_check_key_clave_invalida</t>
+  </si>
+  <si>
+    <t>test_read_key_file_no_fichero</t>
+  </si>
+  <si>
+    <t>test_read_key_file_fichero_mal</t>
+  </si>
+  <si>
+    <t>test_read_key_file_fichero_datos</t>
+  </si>
+  <si>
+    <t>loop_9_times</t>
+  </si>
+  <si>
+    <t>loop_10_times</t>
+  </si>
+  <si>
+    <t>loop_11_times</t>
+  </si>
+  <si>
+    <t>Loop: 3_5_6_(9)_8</t>
+  </si>
+  <si>
+    <t>Loop: 3_5_6_(10)_9</t>
+  </si>
+  <si>
+    <t>Entrar 9 veces (max-1)</t>
+  </si>
+  <si>
+    <t>Entrar 10 veces (max)</t>
+  </si>
+  <si>
+    <t>Entrar 11 veces (max+1)</t>
+  </si>
+  <si>
+    <t>Loop: no se puede</t>
+  </si>
+  <si>
+    <t>Clave valida</t>
+  </si>
+  <si>
+    <t>Clave invalida</t>
+  </si>
+  <si>
+    <t>Fichero formato erroneo</t>
   </si>
 </sst>
 </file>
@@ -195,14 +258,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,7 +401,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G50">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="PATH"/>
@@ -551,17 +613,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.26953125" customWidth="1"/>
     <col min="6" max="7" width="33.7265625" customWidth="1"/>
@@ -596,16 +658,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>5</v>
@@ -616,16 +678,16 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
     </row>
@@ -633,14 +695,14 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -650,165 +712,227 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="4"/>
@@ -817,7 +941,9 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="4"/>
@@ -826,9 +952,11 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="4"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -837,7 +965,7 @@
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="4"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -846,7 +974,7 @@
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="4"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -855,7 +983,7 @@
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="4"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -864,7 +992,7 @@
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="4"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -873,7 +1001,7 @@
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="4"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -882,7 +1010,7 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -891,7 +1019,7 @@
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -900,7 +1028,7 @@
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -909,7 +1037,7 @@
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -918,7 +1046,7 @@
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="4"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -927,7 +1055,7 @@
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="4"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -936,7 +1064,7 @@
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="4"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -945,7 +1073,7 @@
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="4"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -954,7 +1082,7 @@
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="4"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -963,7 +1091,7 @@
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="4"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -972,7 +1100,7 @@
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -981,7 +1109,7 @@
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -990,7 +1118,7 @@
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="4"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -999,7 +1127,7 @@
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="4"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1008,7 +1136,7 @@
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="4"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1017,7 +1145,7 @@
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="C41" s="3"/>
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -1026,7 +1154,7 @@
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="4"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1035,33 +1163,89 @@
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="3"/>
       <c r="D43" s="4"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1998,6 +2182,13 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>